<commit_message>
Actualización desde LENOVO Para Andrea 21-01-2024 07:20
</commit_message>
<xml_diff>
--- a/Resultados/Evaluacion_Documentos.xlsx
+++ b/Resultados/Evaluacion_Documentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\DataPrivacy\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA94571-D0CE-4AB5-8603-8A064B508402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46CDCD1-61EB-46C3-A985-A2C0E513CEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A8DA742-609F-4DE4-93DE-378A477D6C5B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="1304">
   <si>
     <t>Ref</t>
   </si>
@@ -2599,9 +2599,6 @@
   </si>
   <si>
     <t>Alic2023Privacy</t>
-  </si>
-  <si>
-    <t>lo de Conferencia</t>
   </si>
   <si>
     <t>Informatividad del Aviso de Privacidad</t>
@@ -4479,9 +4476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C843FC5-5862-4DB5-AE22-EAB0A5E91C30}">
   <dimension ref="A1:L277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C270" sqref="C270"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.59765625" defaultRowHeight="13.8"/>
@@ -4492,7 +4489,9 @@
     <col min="4" max="4" width="11.59765625" style="4"/>
     <col min="5" max="5" width="22.8984375" style="4" customWidth="1"/>
     <col min="6" max="7" width="27" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="11.59765625" style="4"/>
+    <col min="8" max="11" width="11.59765625" style="4"/>
+    <col min="12" max="12" width="11.59765625" style="1"/>
+    <col min="13" max="16384" width="11.59765625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.6">
@@ -4879,7 +4878,7 @@
       <c r="K10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="1">
         <v>5</v>
       </c>
     </row>
@@ -4918,7 +4917,7 @@
       <c r="K11" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="1">
         <v>5</v>
       </c>
     </row>
@@ -4957,7 +4956,7 @@
       <c r="K12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="1">
         <v>5</v>
       </c>
     </row>
@@ -4996,7 +4995,7 @@
       <c r="K13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5035,7 +5034,7 @@
       <c r="K14" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5074,7 +5073,7 @@
       <c r="K15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5113,7 +5112,7 @@
       <c r="K16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5152,7 +5151,7 @@
       <c r="K17" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5191,7 +5190,7 @@
       <c r="K18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5230,7 +5229,7 @@
       <c r="K19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5269,7 +5268,7 @@
       <c r="K20" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5308,7 +5307,7 @@
       <c r="K21" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5347,7 +5346,7 @@
       <c r="K22" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5386,7 +5385,7 @@
       <c r="K23" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5425,7 +5424,7 @@
       <c r="K24" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5464,7 +5463,7 @@
       <c r="K25" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5503,7 +5502,7 @@
       <c r="K26" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5542,7 +5541,7 @@
       <c r="K27" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5581,7 +5580,7 @@
       <c r="K28" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5620,7 +5619,7 @@
       <c r="K29" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5659,7 +5658,7 @@
       <c r="K30" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5698,7 +5697,7 @@
       <c r="K31" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5737,7 +5736,7 @@
       <c r="K32" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5776,7 +5775,7 @@
       <c r="K33" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5815,7 +5814,7 @@
       <c r="K34" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5854,7 +5853,7 @@
       <c r="K35" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5893,7 +5892,7 @@
       <c r="K36" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36" s="1">
         <v>4</v>
       </c>
     </row>
@@ -5932,7 +5931,7 @@
       <c r="K37" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37" s="1">
         <v>5</v>
       </c>
     </row>
@@ -5971,7 +5970,7 @@
       <c r="K38" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6010,7 +6009,7 @@
       <c r="K39" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6049,7 +6048,7 @@
       <c r="K40" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6088,7 +6087,7 @@
       <c r="K41" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6127,7 +6126,7 @@
       <c r="K42" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6166,7 +6165,7 @@
       <c r="K43" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6205,7 +6204,7 @@
       <c r="K44" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44" s="1">
         <v>4</v>
       </c>
     </row>
@@ -6244,7 +6243,7 @@
       <c r="K45" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45" s="1">
         <v>4</v>
       </c>
     </row>
@@ -6283,7 +6282,7 @@
       <c r="K46" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6322,7 +6321,7 @@
       <c r="K47" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6361,7 +6360,7 @@
       <c r="K48" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6400,7 +6399,7 @@
       <c r="K49" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6439,7 +6438,7 @@
       <c r="K50" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50" s="1">
         <v>4</v>
       </c>
     </row>
@@ -6478,7 +6477,7 @@
       <c r="K51" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6517,7 +6516,7 @@
       <c r="K52" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L52" s="1">
         <v>4</v>
       </c>
     </row>
@@ -6556,7 +6555,7 @@
       <c r="K53" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L53" s="3">
+      <c r="L53" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6595,7 +6594,7 @@
       <c r="K54" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L54" s="3">
+      <c r="L54" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6634,7 +6633,7 @@
       <c r="K55" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="L55" s="3">
+      <c r="L55" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6673,7 +6672,7 @@
       <c r="K56" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="L56" s="3">
+      <c r="L56" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6712,7 +6711,7 @@
       <c r="K57" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L57" s="3">
+      <c r="L57" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6751,7 +6750,7 @@
       <c r="K58" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="L58" s="4">
+      <c r="L58" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6790,7 +6789,7 @@
       <c r="K59" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="L59" s="4">
+      <c r="L59" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6829,7 +6828,7 @@
       <c r="K60" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="L60" s="4">
+      <c r="L60" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6868,7 +6867,7 @@
       <c r="K61" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L61" s="4">
+      <c r="L61" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6907,7 +6906,7 @@
       <c r="K62" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L62" s="4">
+      <c r="L62" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6946,7 +6945,7 @@
       <c r="K63" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L63" s="4">
+      <c r="L63" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6985,7 +6984,7 @@
       <c r="K64" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L64" s="4">
+      <c r="L64" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7024,7 +7023,7 @@
       <c r="K65" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="L65" s="4">
+      <c r="L65" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7063,7 +7062,7 @@
       <c r="K66" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L66" s="4">
+      <c r="L66" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7102,7 +7101,7 @@
       <c r="K67" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="L67" s="4">
+      <c r="L67" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7141,7 +7140,7 @@
       <c r="K68" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="L68" s="4">
+      <c r="L68" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7180,7 +7179,7 @@
       <c r="K69" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L69" s="4">
+      <c r="L69" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7219,7 +7218,7 @@
       <c r="K70" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="L70" s="4">
+      <c r="L70" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7258,7 +7257,7 @@
       <c r="K71" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="L71" s="4">
+      <c r="L71" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7297,7 +7296,7 @@
       <c r="K72" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L72" s="4">
+      <c r="L72" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7336,7 +7335,7 @@
       <c r="K73" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L73" s="4">
+      <c r="L73" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7375,7 +7374,7 @@
       <c r="K74" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="L74" s="3">
+      <c r="L74" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7414,7 +7413,7 @@
       <c r="K75" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L75" s="3">
+      <c r="L75" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7453,7 +7452,7 @@
       <c r="K76" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="L76" s="3">
+      <c r="L76" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7492,7 +7491,7 @@
       <c r="K77" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="L77" s="3">
+      <c r="L77" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7531,7 +7530,7 @@
       <c r="K78" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L78" s="3">
+      <c r="L78" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7570,7 +7569,7 @@
       <c r="K79" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="L79" s="3">
+      <c r="L79" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7609,7 +7608,7 @@
       <c r="K80" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="L80" s="3">
+      <c r="L80" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7648,7 +7647,7 @@
       <c r="K81" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="L81" s="3">
+      <c r="L81" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7687,7 +7686,7 @@
       <c r="K82" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="L82" s="3">
+      <c r="L82" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7726,7 +7725,7 @@
       <c r="K83" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L83" s="3">
+      <c r="L83" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7765,7 +7764,7 @@
       <c r="K84" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L84" s="3">
+      <c r="L84" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7804,7 +7803,7 @@
       <c r="K85" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="L85" s="3">
+      <c r="L85" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7843,7 +7842,7 @@
       <c r="K86" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="L86" s="3">
+      <c r="L86" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7882,7 +7881,7 @@
       <c r="K87" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="L87" s="3">
+      <c r="L87" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7921,7 +7920,7 @@
       <c r="K88" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="L88" s="3">
+      <c r="L88" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7960,7 +7959,7 @@
       <c r="K89" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="L89" s="3">
+      <c r="L89" s="1">
         <v>5</v>
       </c>
     </row>
@@ -7999,7 +7998,7 @@
       <c r="K90" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="L90" s="3">
+      <c r="L90" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8038,7 +8037,7 @@
       <c r="K91" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="L91" s="3">
+      <c r="L91" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8077,7 +8076,7 @@
       <c r="K92" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="L92" s="3">
+      <c r="L92" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8116,7 +8115,7 @@
       <c r="K93" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="L93" s="3">
+      <c r="L93" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8155,7 +8154,7 @@
       <c r="K94" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="L94" s="3">
+      <c r="L94" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8194,7 +8193,7 @@
       <c r="K95" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="L95" s="3">
+      <c r="L95" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8233,7 +8232,7 @@
       <c r="K96" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="L96" s="3">
+      <c r="L96" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8272,7 +8271,7 @@
       <c r="K97" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="L97" s="3">
+      <c r="L97" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8311,7 +8310,7 @@
       <c r="K98" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="L98" s="3">
+      <c r="L98" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8350,7 +8349,7 @@
       <c r="K99" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="L99" s="3">
+      <c r="L99" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8389,7 +8388,7 @@
       <c r="K100" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="L100" s="3">
+      <c r="L100" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8428,7 +8427,7 @@
       <c r="K101" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="L101" s="3">
+      <c r="L101" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8467,7 +8466,7 @@
       <c r="K102" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="L102" s="3">
+      <c r="L102" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8506,7 +8505,7 @@
       <c r="K103" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="L103" s="3">
+      <c r="L103" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8545,7 +8544,7 @@
       <c r="K104" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="L104" s="3">
+      <c r="L104" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8584,7 +8583,7 @@
       <c r="K105" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="L105" s="3">
+      <c r="L105" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8623,7 +8622,7 @@
       <c r="K106" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L106" s="3">
+      <c r="L106" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8662,7 +8661,7 @@
       <c r="K107" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="L107" s="3">
+      <c r="L107" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8701,7 +8700,7 @@
       <c r="K108" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="L108" s="3">
+      <c r="L108" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8740,7 +8739,7 @@
       <c r="K109" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L109" s="3">
+      <c r="L109" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8779,7 +8778,7 @@
       <c r="K110" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L110" s="3">
+      <c r="L110" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8818,7 +8817,7 @@
       <c r="K111" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="L111" s="3">
+      <c r="L111" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8857,7 +8856,7 @@
       <c r="K112" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L112" s="3">
+      <c r="L112" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8896,7 +8895,7 @@
       <c r="K113" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L113" s="3">
+      <c r="L113" s="1">
         <v>5</v>
       </c>
     </row>
@@ -8935,7 +8934,7 @@
       <c r="K114" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="L114" s="3">
+      <c r="L114" s="1">
         <v>3</v>
       </c>
     </row>
@@ -8974,7 +8973,7 @@
       <c r="K115" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L115" s="3">
+      <c r="L115" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9013,7 +9012,7 @@
       <c r="K116" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="L116" s="3">
+      <c r="L116" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9052,7 +9051,7 @@
       <c r="K117" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L117" s="3">
+      <c r="L117" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9091,7 +9090,7 @@
       <c r="K118" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L118" s="3">
+      <c r="L118" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9130,7 +9129,7 @@
       <c r="K119" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L119" s="3">
+      <c r="L119" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9169,7 +9168,7 @@
       <c r="K120" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="L120" s="3">
+      <c r="L120" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9208,7 +9207,7 @@
       <c r="K121" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L121" s="3">
+      <c r="L121" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9247,7 +9246,7 @@
       <c r="K122" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="L122" s="3">
+      <c r="L122" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9286,7 +9285,7 @@
       <c r="K123" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="L123" s="3">
+      <c r="L123" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9325,7 +9324,7 @@
       <c r="K124" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L124" s="3">
+      <c r="L124" s="1">
         <v>4</v>
       </c>
     </row>
@@ -9364,7 +9363,7 @@
       <c r="K125" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L125" s="3">
+      <c r="L125" s="1">
         <v>4</v>
       </c>
     </row>
@@ -9403,7 +9402,7 @@
       <c r="K126" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="L126" s="3">
+      <c r="L126" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9442,7 +9441,7 @@
       <c r="K127" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L127" s="3">
+      <c r="L127" s="1">
         <v>4</v>
       </c>
     </row>
@@ -9481,7 +9480,7 @@
       <c r="K128" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L128" s="3">
+      <c r="L128" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9520,7 +9519,7 @@
       <c r="K129" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L129" s="3">
+      <c r="L129" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9559,7 +9558,7 @@
       <c r="K130" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L130" s="3">
+      <c r="L130" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9598,7 +9597,7 @@
       <c r="K131" s="3" t="s">
         <v>687</v>
       </c>
-      <c r="L131" s="3">
+      <c r="L131" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9637,7 +9636,7 @@
       <c r="K132" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L132" s="3">
+      <c r="L132" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9676,7 +9675,7 @@
       <c r="K133" s="3" t="s">
         <v>698</v>
       </c>
-      <c r="L133" s="3">
+      <c r="L133" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9715,7 +9714,7 @@
       <c r="K134" s="3" t="s">
         <v>702</v>
       </c>
-      <c r="L134" s="3">
+      <c r="L134" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9754,7 +9753,7 @@
       <c r="K135" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L135" s="3">
+      <c r="L135" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9793,7 +9792,7 @@
       <c r="K136" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L136" s="3">
+      <c r="L136" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9832,7 +9831,7 @@
       <c r="K137" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L137" s="3">
+      <c r="L137" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9871,7 +9870,7 @@
       <c r="K138" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L138" s="3">
+      <c r="L138" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9910,7 +9909,7 @@
       <c r="K139" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L139" s="3">
+      <c r="L139" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9949,7 +9948,7 @@
       <c r="K140" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="L140" s="3">
+      <c r="L140" s="1">
         <v>5</v>
       </c>
     </row>
@@ -9988,7 +9987,7 @@
       <c r="K141" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="L141" s="3">
+      <c r="L141" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10027,7 +10026,7 @@
       <c r="K142" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="L142" s="3">
+      <c r="L142" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10066,7 +10065,7 @@
       <c r="K143" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L143" s="3">
+      <c r="L143" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10105,7 +10104,7 @@
       <c r="K144" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L144" s="3">
+      <c r="L144" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10144,7 +10143,7 @@
       <c r="K145" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="L145" s="3">
+      <c r="L145" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10183,7 +10182,7 @@
       <c r="K146" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="L146" s="3">
+      <c r="L146" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10222,7 +10221,7 @@
       <c r="K147" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="L147" s="3">
+      <c r="L147" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10261,7 +10260,7 @@
       <c r="K148" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L148" s="3">
+      <c r="L148" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10300,7 +10299,7 @@
       <c r="K149" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="L149" s="3">
+      <c r="L149" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10339,7 +10338,7 @@
       <c r="K150" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L150" s="3">
+      <c r="L150" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10378,7 +10377,7 @@
       <c r="K151" s="3" t="s">
         <v>792</v>
       </c>
-      <c r="L151" s="3">
+      <c r="L151" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10417,7 +10416,7 @@
       <c r="K152" s="3" t="s">
         <v>796</v>
       </c>
-      <c r="L152" s="3">
+      <c r="L152" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10429,8 +10428,8 @@
       <c r="B153" s="3" t="s">
         <v>798</v>
       </c>
-      <c r="C153" s="3" t="s">
-        <v>11</v>
+      <c r="C153" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="D153" s="3">
         <v>2022</v>
@@ -10456,7 +10455,7 @@
       <c r="K153" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L153" s="3">
+      <c r="L153" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10495,7 +10494,7 @@
       <c r="K154" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L154" s="3">
+      <c r="L154" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10534,7 +10533,7 @@
       <c r="K155" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L155" s="3">
+      <c r="L155" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10573,7 +10572,7 @@
       <c r="K156" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="L156" s="3">
+      <c r="L156" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10612,7 +10611,7 @@
       <c r="K157" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="L157" s="3">
+      <c r="L157" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10651,7 +10650,7 @@
       <c r="K158" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L158" s="3">
+      <c r="L158" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10690,7 +10689,7 @@
       <c r="K159" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="L159" s="3">
+      <c r="L159" s="1">
         <v>5</v>
       </c>
     </row>
@@ -10792,26 +10791,26 @@
       <c r="B163" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="C163" s="19" t="s">
-        <v>855</v>
+      <c r="C163" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D163" s="19">
         <v>2023</v>
       </c>
       <c r="E163" s="19" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F163" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G163" s="19" t="s">
+        <v>856</v>
+      </c>
+      <c r="H163" s="19" t="s">
         <v>857</v>
       </c>
-      <c r="H163" s="19" t="s">
+      <c r="I163" s="19" t="s">
         <v>858</v>
-      </c>
-      <c r="I163" s="19" t="s">
-        <v>859</v>
       </c>
       <c r="J163" s="19">
         <v>4</v>
@@ -10822,28 +10821,28 @@
     </row>
     <row r="164" spans="2:11" ht="51.6" thickBot="1">
       <c r="B164" s="21" t="s">
-        <v>860</v>
-      </c>
-      <c r="C164" s="19" t="s">
-        <v>861</v>
+        <v>859</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D164" s="19">
         <v>2022</v>
       </c>
       <c r="E164" s="19" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F164" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G164" s="19" t="s">
+        <v>862</v>
+      </c>
+      <c r="H164" s="19" t="s">
         <v>863</v>
       </c>
-      <c r="H164" s="19" t="s">
+      <c r="I164" s="19" t="s">
         <v>864</v>
-      </c>
-      <c r="I164" s="19" t="s">
-        <v>865</v>
       </c>
       <c r="J164" s="19">
         <v>4</v>
@@ -10854,7 +10853,7 @@
     </row>
     <row r="165" spans="2:11" ht="51.6" thickBot="1">
       <c r="B165" s="21" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>135</v>
@@ -10863,13 +10862,13 @@
         <v>2022</v>
       </c>
       <c r="E165" s="19" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F165" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G165" s="19" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H165" s="19" t="s">
         <v>133</v>
@@ -10886,7 +10885,7 @@
     </row>
     <row r="166" spans="2:11" ht="51.6" thickBot="1">
       <c r="B166" s="21" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>135</v>
@@ -10895,13 +10894,13 @@
         <v>2021</v>
       </c>
       <c r="E166" s="19" t="s">
+        <v>869</v>
+      </c>
+      <c r="F166" s="19" t="s">
         <v>870</v>
       </c>
-      <c r="F166" s="19" t="s">
+      <c r="G166" s="19" t="s">
         <v>871</v>
-      </c>
-      <c r="G166" s="19" t="s">
-        <v>872</v>
       </c>
       <c r="H166" s="19" t="s">
         <v>133</v>
@@ -10927,19 +10926,19 @@
         <v>2023</v>
       </c>
       <c r="E167" s="19" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F167" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G167" s="19" t="s">
+        <v>873</v>
+      </c>
+      <c r="H167" s="19" t="s">
         <v>874</v>
       </c>
-      <c r="H167" s="19" t="s">
+      <c r="I167" s="19" t="s">
         <v>875</v>
-      </c>
-      <c r="I167" s="19" t="s">
-        <v>876</v>
       </c>
       <c r="J167" s="20">
         <v>5</v>
@@ -10950,7 +10949,7 @@
     </row>
     <row r="168" spans="2:11" ht="41.4" thickBot="1">
       <c r="B168" s="21" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C168" s="19" t="s">
         <v>851</v>
@@ -10959,16 +10958,16 @@
         <v>2022</v>
       </c>
       <c r="E168" s="19" t="s">
+        <v>877</v>
+      </c>
+      <c r="F168" s="19" t="s">
         <v>878</v>
       </c>
-      <c r="F168" s="19" t="s">
+      <c r="G168" s="19" t="s">
         <v>879</v>
       </c>
-      <c r="G168" s="19" t="s">
+      <c r="H168" s="19" t="s">
         <v>880</v>
-      </c>
-      <c r="H168" s="19" t="s">
-        <v>881</v>
       </c>
       <c r="I168" s="19" t="s">
         <v>845</v>
@@ -10982,7 +10981,7 @@
     </row>
     <row r="169" spans="2:11" ht="31.2" thickBot="1">
       <c r="B169" s="21" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>18</v>
@@ -10991,16 +10990,16 @@
         <v>2022</v>
       </c>
       <c r="E169" s="21" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="F169" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G169" s="19" t="s">
+        <v>883</v>
+      </c>
+      <c r="H169" s="19" t="s">
         <v>884</v>
-      </c>
-      <c r="H169" s="19" t="s">
-        <v>885</v>
       </c>
       <c r="I169" s="19" t="s">
         <v>845</v>
@@ -11014,7 +11013,7 @@
     </row>
     <row r="170" spans="2:11" ht="31.2" thickBot="1">
       <c r="B170" s="12" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>135</v>
@@ -11023,19 +11022,19 @@
         <v>2019</v>
       </c>
       <c r="E170" s="10" t="s">
+        <v>886</v>
+      </c>
+      <c r="F170" s="8" t="s">
         <v>887</v>
       </c>
-      <c r="F170" s="8" t="s">
+      <c r="G170" s="8" t="s">
         <v>888</v>
       </c>
-      <c r="G170" s="8" t="s">
+      <c r="H170" s="8" t="s">
         <v>889</v>
       </c>
-      <c r="H170" s="8" t="s">
+      <c r="I170" s="8" t="s">
         <v>890</v>
-      </c>
-      <c r="I170" s="8" t="s">
-        <v>891</v>
       </c>
       <c r="J170" s="8">
         <v>5</v>
@@ -11046,25 +11045,25 @@
     </row>
     <row r="171" spans="2:11" ht="41.4" thickBot="1">
       <c r="B171" s="12" t="s">
+        <v>891</v>
+      </c>
+      <c r="C171" s="8" t="s">
         <v>892</v>
-      </c>
-      <c r="C171" s="8" t="s">
-        <v>893</v>
       </c>
       <c r="D171" s="8">
         <v>2022</v>
       </c>
       <c r="E171" s="8" t="s">
+        <v>893</v>
+      </c>
+      <c r="F171" s="8" t="s">
         <v>894</v>
       </c>
-      <c r="F171" s="8" t="s">
+      <c r="G171" s="8" t="s">
         <v>895</v>
       </c>
-      <c r="G171" s="8" t="s">
+      <c r="H171" s="8" t="s">
         <v>896</v>
-      </c>
-      <c r="H171" s="8" t="s">
-        <v>897</v>
       </c>
       <c r="I171" s="8" t="s">
         <v>845</v>
@@ -11078,7 +11077,7 @@
     </row>
     <row r="172" spans="2:11" ht="41.4" thickBot="1">
       <c r="B172" s="12" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>18</v>
@@ -11087,16 +11086,16 @@
         <v>2019</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="F172" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G172" s="8" t="s">
+        <v>899</v>
+      </c>
+      <c r="H172" s="8" t="s">
         <v>900</v>
-      </c>
-      <c r="H172" s="8" t="s">
-        <v>901</v>
       </c>
       <c r="I172" s="8" t="s">
         <v>845</v>
@@ -11110,7 +11109,7 @@
     </row>
     <row r="173" spans="2:11" ht="41.4" thickBot="1">
       <c r="B173" s="12" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>18</v>
@@ -11119,16 +11118,16 @@
         <v>2022</v>
       </c>
       <c r="E173" s="8" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F173" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G173" s="8" t="s">
+        <v>903</v>
+      </c>
+      <c r="H173" s="8" t="s">
         <v>904</v>
-      </c>
-      <c r="H173" s="8" t="s">
-        <v>905</v>
       </c>
       <c r="I173" s="8" t="s">
         <v>845</v>
@@ -11142,7 +11141,7 @@
     </row>
     <row r="174" spans="2:11" ht="41.4" thickBot="1">
       <c r="B174" s="12" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>18</v>
@@ -11151,16 +11150,16 @@
         <v>2022</v>
       </c>
       <c r="E174" s="8" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F174" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G174" s="8" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="H174" s="8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I174" s="8" t="s">
         <v>845</v>
@@ -11174,7 +11173,7 @@
     </row>
     <row r="175" spans="2:11" ht="41.4" thickBot="1">
       <c r="B175" s="12" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>135</v>
@@ -11183,19 +11182,19 @@
         <v>2024</v>
       </c>
       <c r="E175" s="8" t="s">
+        <v>909</v>
+      </c>
+      <c r="F175" s="8" t="s">
         <v>910</v>
       </c>
-      <c r="F175" s="8" t="s">
+      <c r="G175" s="8" t="s">
         <v>911</v>
       </c>
-      <c r="G175" s="8" t="s">
+      <c r="H175" s="8" t="s">
         <v>912</v>
       </c>
-      <c r="H175" s="8" t="s">
-        <v>913</v>
-      </c>
       <c r="I175" s="8" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J175" s="8">
         <v>4</v>
@@ -11206,7 +11205,7 @@
     </row>
     <row r="176" spans="2:11" ht="51.6" thickBot="1">
       <c r="B176" s="12" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>135</v>
@@ -11215,16 +11214,16 @@
         <v>2021</v>
       </c>
       <c r="E176" s="8" t="s">
+        <v>914</v>
+      </c>
+      <c r="F176" s="8" t="s">
         <v>915</v>
       </c>
-      <c r="F176" s="8" t="s">
+      <c r="G176" s="8" t="s">
         <v>916</v>
       </c>
-      <c r="G176" s="8" t="s">
+      <c r="H176" s="8" t="s">
         <v>917</v>
-      </c>
-      <c r="H176" s="8" t="s">
-        <v>918</v>
       </c>
       <c r="I176" s="8" t="s">
         <v>845</v>
@@ -11238,7 +11237,7 @@
     </row>
     <row r="177" spans="2:11" ht="41.4" thickBot="1">
       <c r="B177" s="12" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>135</v>
@@ -11247,16 +11246,16 @@
         <v>2022</v>
       </c>
       <c r="E177" s="8" t="s">
+        <v>919</v>
+      </c>
+      <c r="F177" s="8" t="s">
         <v>920</v>
       </c>
-      <c r="F177" s="8" t="s">
+      <c r="G177" s="8" t="s">
         <v>921</v>
       </c>
-      <c r="G177" s="8" t="s">
+      <c r="H177" s="8" t="s">
         <v>922</v>
-      </c>
-      <c r="H177" s="8" t="s">
-        <v>923</v>
       </c>
       <c r="I177" s="8" t="s">
         <v>845</v>
@@ -11270,7 +11269,7 @@
     </row>
     <row r="178" spans="2:11" ht="41.4" thickBot="1">
       <c r="B178" s="22" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>18</v>
@@ -11279,19 +11278,19 @@
         <v>2019</v>
       </c>
       <c r="E178" s="18" t="s">
+        <v>924</v>
+      </c>
+      <c r="F178" s="18" t="s">
         <v>925</v>
       </c>
-      <c r="F178" s="18" t="s">
+      <c r="G178" s="18" t="s">
         <v>926</v>
       </c>
-      <c r="G178" s="18" t="s">
+      <c r="H178" s="18" t="s">
         <v>927</v>
       </c>
-      <c r="H178" s="18" t="s">
-        <v>928</v>
-      </c>
       <c r="I178" s="8" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J178" s="18">
         <v>5</v>
@@ -11302,7 +11301,7 @@
     </row>
     <row r="179" spans="2:11" ht="51.6" thickBot="1">
       <c r="B179" s="22" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>18</v>
@@ -11311,19 +11310,19 @@
         <v>2023</v>
       </c>
       <c r="E179" s="18" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F179" s="18" t="s">
         <v>20</v>
       </c>
       <c r="G179" s="18" t="s">
+        <v>930</v>
+      </c>
+      <c r="H179" s="18" t="s">
         <v>931</v>
       </c>
-      <c r="H179" s="18" t="s">
-        <v>932</v>
-      </c>
       <c r="I179" s="8" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J179" s="18">
         <v>5</v>
@@ -11334,7 +11333,7 @@
     </row>
     <row r="180" spans="2:11" ht="36.6" customHeight="1" thickBot="1">
       <c r="B180" s="21" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>135</v>
@@ -11343,16 +11342,16 @@
         <v>2021</v>
       </c>
       <c r="E180" s="19" t="s">
+        <v>933</v>
+      </c>
+      <c r="F180" s="19" t="s">
         <v>934</v>
       </c>
-      <c r="F180" s="19" t="s">
+      <c r="G180" s="19" t="s">
         <v>935</v>
       </c>
-      <c r="G180" s="19" t="s">
+      <c r="H180" s="19" t="s">
         <v>936</v>
-      </c>
-      <c r="H180" s="19" t="s">
-        <v>937</v>
       </c>
       <c r="I180" s="13" t="s">
         <v>845</v>
@@ -11366,7 +11365,7 @@
     </row>
     <row r="181" spans="2:11" ht="51.6" thickBot="1">
       <c r="B181" s="14" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>135</v>
@@ -11375,16 +11374,16 @@
         <v>2020</v>
       </c>
       <c r="E181" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="F181" s="13" t="s">
         <v>939</v>
       </c>
-      <c r="F181" s="13" t="s">
+      <c r="G181" s="13" t="s">
         <v>940</v>
       </c>
-      <c r="G181" s="13" t="s">
+      <c r="H181" s="13" t="s">
         <v>941</v>
-      </c>
-      <c r="H181" s="13" t="s">
-        <v>942</v>
       </c>
       <c r="I181" s="13" t="s">
         <v>845</v>
@@ -11398,7 +11397,7 @@
     </row>
     <row r="182" spans="2:11" ht="51.6" thickBot="1">
       <c r="B182" s="14" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>135</v>
@@ -11407,16 +11406,16 @@
         <v>2021</v>
       </c>
       <c r="E182" s="13" t="s">
+        <v>943</v>
+      </c>
+      <c r="F182" s="13" t="s">
         <v>944</v>
       </c>
-      <c r="F182" s="13" t="s">
+      <c r="G182" s="13" t="s">
         <v>945</v>
       </c>
-      <c r="G182" s="13" t="s">
+      <c r="H182" s="13" t="s">
         <v>946</v>
-      </c>
-      <c r="H182" s="13" t="s">
-        <v>947</v>
       </c>
       <c r="I182" s="13" t="s">
         <v>845</v>
@@ -11430,7 +11429,7 @@
     </row>
     <row r="183" spans="2:11" ht="61.8" thickBot="1">
       <c r="B183" s="14" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C183" s="13" t="s">
         <v>851</v>
@@ -11439,16 +11438,16 @@
         <v>2024</v>
       </c>
       <c r="E183" s="13" t="s">
+        <v>948</v>
+      </c>
+      <c r="F183" s="13" t="s">
         <v>949</v>
       </c>
-      <c r="F183" s="13" t="s">
+      <c r="G183" s="13" t="s">
         <v>950</v>
       </c>
-      <c r="G183" s="13" t="s">
+      <c r="H183" s="13" t="s">
         <v>951</v>
-      </c>
-      <c r="H183" s="13" t="s">
-        <v>952</v>
       </c>
       <c r="I183" s="13" t="s">
         <v>845</v>
@@ -11462,7 +11461,7 @@
     </row>
     <row r="184" spans="2:11" ht="66" customHeight="1" thickBot="1">
       <c r="B184" s="14" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>135</v>
@@ -11471,19 +11470,19 @@
         <v>2022</v>
       </c>
       <c r="E184" s="13" t="s">
+        <v>953</v>
+      </c>
+      <c r="F184" s="13" t="s">
         <v>954</v>
       </c>
-      <c r="F184" s="13" t="s">
+      <c r="G184" s="13" t="s">
         <v>955</v>
       </c>
-      <c r="G184" s="13" t="s">
+      <c r="H184" s="13" t="s">
         <v>956</v>
       </c>
-      <c r="H184" s="13" t="s">
-        <v>957</v>
-      </c>
       <c r="I184" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J184" s="13">
         <v>5</v>
@@ -11494,7 +11493,7 @@
     </row>
     <row r="185" spans="2:11" ht="61.8" thickBot="1">
       <c r="B185" s="14" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>135</v>
@@ -11503,16 +11502,16 @@
         <v>2023</v>
       </c>
       <c r="E185" s="13" t="s">
+        <v>958</v>
+      </c>
+      <c r="F185" s="13" t="s">
+        <v>939</v>
+      </c>
+      <c r="G185" s="13" t="s">
         <v>959</v>
       </c>
-      <c r="F185" s="13" t="s">
-        <v>940</v>
-      </c>
-      <c r="G185" s="13" t="s">
+      <c r="H185" s="13" t="s">
         <v>960</v>
-      </c>
-      <c r="H185" s="13" t="s">
-        <v>961</v>
       </c>
       <c r="I185" s="13" t="s">
         <v>845</v>
@@ -11526,7 +11525,7 @@
     </row>
     <row r="186" spans="2:11" ht="51.6" thickBot="1">
       <c r="B186" s="14" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C186" s="13" t="s">
         <v>54</v>
@@ -11535,16 +11534,16 @@
         <v>2024</v>
       </c>
       <c r="E186" s="13" t="s">
+        <v>962</v>
+      </c>
+      <c r="F186" s="13" t="s">
+        <v>949</v>
+      </c>
+      <c r="G186" s="13" t="s">
         <v>963</v>
       </c>
-      <c r="F186" s="13" t="s">
-        <v>950</v>
-      </c>
-      <c r="G186" s="13" t="s">
+      <c r="H186" s="13" t="s">
         <v>964</v>
-      </c>
-      <c r="H186" s="13" t="s">
-        <v>965</v>
       </c>
       <c r="I186" s="13" t="s">
         <v>845</v>
@@ -11558,25 +11557,25 @@
     </row>
     <row r="187" spans="2:11" ht="51.6" thickBot="1">
       <c r="B187" s="14" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C187" s="13" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D187" s="13">
         <v>2019</v>
       </c>
       <c r="E187" s="13" t="s">
+        <v>966</v>
+      </c>
+      <c r="F187" s="13" t="s">
+        <v>939</v>
+      </c>
+      <c r="G187" s="13" t="s">
         <v>967</v>
       </c>
-      <c r="F187" s="13" t="s">
-        <v>940</v>
-      </c>
-      <c r="G187" s="13" t="s">
+      <c r="H187" s="13" t="s">
         <v>968</v>
-      </c>
-      <c r="H187" s="13" t="s">
-        <v>969</v>
       </c>
       <c r="I187" s="13" t="s">
         <v>845</v>
@@ -11590,25 +11589,25 @@
     </row>
     <row r="188" spans="2:11" ht="51.6" thickBot="1">
       <c r="B188" s="14" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C188" s="13" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D188" s="13">
         <v>2022</v>
       </c>
       <c r="E188" s="13" t="s">
+        <v>970</v>
+      </c>
+      <c r="F188" s="13" t="s">
         <v>971</v>
       </c>
-      <c r="F188" s="13" t="s">
+      <c r="G188" s="13" t="s">
         <v>972</v>
       </c>
-      <c r="G188" s="13" t="s">
+      <c r="H188" s="13" t="s">
         <v>973</v>
-      </c>
-      <c r="H188" s="13" t="s">
-        <v>974</v>
       </c>
       <c r="I188" s="13" t="s">
         <v>845</v>
@@ -11622,28 +11621,28 @@
     </row>
     <row r="189" spans="2:11" ht="21" thickBot="1">
       <c r="B189" s="14" t="s">
+        <v>974</v>
+      </c>
+      <c r="C189" s="13" t="s">
         <v>975</v>
-      </c>
-      <c r="C189" s="13" t="s">
-        <v>976</v>
       </c>
       <c r="D189" s="13">
         <v>2019</v>
       </c>
       <c r="E189" s="13" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F189" s="13" t="s">
         <v>216</v>
       </c>
       <c r="G189" s="13" t="s">
+        <v>977</v>
+      </c>
+      <c r="H189" s="13" t="s">
         <v>978</v>
       </c>
-      <c r="H189" s="13" t="s">
-        <v>979</v>
-      </c>
       <c r="I189" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J189" s="13">
         <v>5</v>
@@ -11654,7 +11653,7 @@
     </row>
     <row r="190" spans="2:11" ht="41.4" thickBot="1">
       <c r="B190" s="14" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C190" s="13" t="s">
         <v>851</v>
@@ -11663,13 +11662,13 @@
         <v>2016</v>
       </c>
       <c r="E190" s="13" t="s">
+        <v>980</v>
+      </c>
+      <c r="F190" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G190" s="13" t="s">
         <v>981</v>
-      </c>
-      <c r="F190" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G190" s="13" t="s">
-        <v>982</v>
       </c>
       <c r="H190" s="13" t="s">
         <v>133</v>
@@ -11686,7 +11685,7 @@
     </row>
     <row r="191" spans="2:11" ht="31.2" thickBot="1">
       <c r="B191" s="14" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C191" s="13" t="s">
         <v>851</v>
@@ -11695,19 +11694,19 @@
         <v>2024</v>
       </c>
       <c r="E191" s="13" t="s">
+        <v>983</v>
+      </c>
+      <c r="F191" s="13" t="s">
         <v>984</v>
       </c>
-      <c r="F191" s="13" t="s">
+      <c r="G191" s="13" t="s">
         <v>985</v>
-      </c>
-      <c r="G191" s="13" t="s">
-        <v>986</v>
       </c>
       <c r="H191" s="13" t="s">
         <v>133</v>
       </c>
       <c r="I191" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J191" s="13">
         <v>5</v>
@@ -11718,22 +11717,22 @@
     </row>
     <row r="192" spans="2:11" ht="51.6" thickBot="1">
       <c r="B192" s="14" t="s">
+        <v>986</v>
+      </c>
+      <c r="C192" s="13" t="s">
         <v>987</v>
-      </c>
-      <c r="C192" s="13" t="s">
-        <v>988</v>
       </c>
       <c r="D192" s="13">
         <v>2023</v>
       </c>
       <c r="E192" s="13" t="s">
+        <v>988</v>
+      </c>
+      <c r="F192" s="13" t="s">
         <v>989</v>
       </c>
-      <c r="F192" s="13" t="s">
+      <c r="G192" s="13" t="s">
         <v>990</v>
-      </c>
-      <c r="G192" s="13" t="s">
-        <v>991</v>
       </c>
       <c r="H192" s="13" t="s">
         <v>139</v>
@@ -11750,7 +11749,7 @@
     </row>
     <row r="193" spans="2:11" ht="31.2" thickBot="1">
       <c r="B193" s="14" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>18</v>
@@ -11759,16 +11758,16 @@
         <v>2020</v>
       </c>
       <c r="E193" s="13" t="s">
+        <v>992</v>
+      </c>
+      <c r="F193" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G193" s="13" t="s">
         <v>993</v>
       </c>
-      <c r="F193" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G193" s="13" t="s">
+      <c r="H193" s="13" t="s">
         <v>994</v>
-      </c>
-      <c r="H193" s="13" t="s">
-        <v>995</v>
       </c>
       <c r="I193" s="13" t="s">
         <v>845</v>
@@ -11782,7 +11781,7 @@
     </row>
     <row r="194" spans="2:11" ht="41.4" thickBot="1">
       <c r="B194" s="14" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>135</v>
@@ -11791,19 +11790,19 @@
         <v>2022</v>
       </c>
       <c r="E194" s="13" t="s">
+        <v>996</v>
+      </c>
+      <c r="F194" s="13" t="s">
         <v>997</v>
       </c>
-      <c r="F194" s="13" t="s">
+      <c r="G194" s="13" t="s">
         <v>998</v>
-      </c>
-      <c r="G194" s="13" t="s">
-        <v>999</v>
       </c>
       <c r="H194" s="13" t="s">
         <v>133</v>
       </c>
       <c r="I194" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J194" s="13">
         <v>5</v>
@@ -11814,7 +11813,7 @@
     </row>
     <row r="195" spans="2:11" ht="41.4" thickBot="1">
       <c r="B195" s="14" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>18</v>
@@ -11823,13 +11822,13 @@
         <v>2023</v>
       </c>
       <c r="E195" s="13" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F195" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G195" s="13" t="s">
         <v>1001</v>
-      </c>
-      <c r="F195" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G195" s="13" t="s">
-        <v>1002</v>
       </c>
       <c r="H195" s="13" t="s">
         <v>133</v>
@@ -11846,7 +11845,7 @@
     </row>
     <row r="196" spans="2:11" ht="61.8" thickBot="1">
       <c r="B196" s="14" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>135</v>
@@ -11855,19 +11854,19 @@
         <v>2022</v>
       </c>
       <c r="E196" s="13" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F196" s="13" t="s">
+        <v>989</v>
+      </c>
+      <c r="G196" s="13" t="s">
         <v>1004</v>
-      </c>
-      <c r="F196" s="13" t="s">
-        <v>990</v>
-      </c>
-      <c r="G196" s="13" t="s">
-        <v>1005</v>
       </c>
       <c r="H196" s="13" t="s">
         <v>133</v>
       </c>
       <c r="I196" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J196" s="13">
         <v>5</v>
@@ -11878,7 +11877,7 @@
     </row>
     <row r="197" spans="2:11" ht="31.2" thickBot="1">
       <c r="B197" s="14" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>18</v>
@@ -11887,19 +11886,19 @@
         <v>2024</v>
       </c>
       <c r="E197" s="13" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F197" s="13" t="s">
         <v>1007</v>
       </c>
-      <c r="F197" s="13" t="s">
+      <c r="G197" s="13" t="s">
         <v>1008</v>
-      </c>
-      <c r="G197" s="13" t="s">
-        <v>1009</v>
       </c>
       <c r="H197" s="13" t="s">
         <v>131</v>
       </c>
       <c r="I197" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J197" s="13">
         <v>5</v>
@@ -11910,7 +11909,7 @@
     </row>
     <row r="198" spans="2:11" ht="31.2" thickBot="1">
       <c r="B198" s="14" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C198" s="13" t="s">
         <v>851</v>
@@ -11919,13 +11918,13 @@
         <v>2023</v>
       </c>
       <c r="E198" s="13" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F198" s="13" t="s">
+        <v>984</v>
+      </c>
+      <c r="G198" s="13" t="s">
         <v>1011</v>
-      </c>
-      <c r="F198" s="13" t="s">
-        <v>985</v>
-      </c>
-      <c r="G198" s="13" t="s">
-        <v>1012</v>
       </c>
       <c r="H198" s="13" t="s">
         <v>133</v>
@@ -11942,7 +11941,7 @@
     </row>
     <row r="199" spans="2:11" ht="31.2" thickBot="1">
       <c r="B199" s="14" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>18</v>
@@ -11951,13 +11950,13 @@
         <v>2019</v>
       </c>
       <c r="E199" s="13" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F199" s="13" t="s">
         <v>1014</v>
       </c>
-      <c r="F199" s="13" t="s">
+      <c r="G199" s="13" t="s">
         <v>1015</v>
-      </c>
-      <c r="G199" s="13" t="s">
-        <v>1016</v>
       </c>
       <c r="H199" s="13" t="s">
         <v>133</v>
@@ -11974,25 +11973,25 @@
     </row>
     <row r="200" spans="2:11" ht="41.4" thickBot="1">
       <c r="B200" s="14" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C200" s="13" t="s">
         <v>1017</v>
-      </c>
-      <c r="C200" s="13" t="s">
-        <v>1018</v>
       </c>
       <c r="D200" s="13">
         <v>2021</v>
       </c>
       <c r="E200" s="13" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F200" s="13" t="s">
         <v>1019</v>
       </c>
-      <c r="F200" s="13" t="s">
+      <c r="G200" s="13" t="s">
         <v>1020</v>
       </c>
-      <c r="G200" s="13" t="s">
+      <c r="H200" s="13" t="s">
         <v>1021</v>
-      </c>
-      <c r="H200" s="13" t="s">
-        <v>1022</v>
       </c>
       <c r="I200" s="13" t="s">
         <v>845</v>
@@ -12006,7 +12005,7 @@
     </row>
     <row r="201" spans="2:11" ht="31.2" thickBot="1">
       <c r="B201" s="14" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>18</v>
@@ -12015,13 +12014,13 @@
         <v>2019</v>
       </c>
       <c r="E201" s="13" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F201" s="13" t="s">
+        <v>994</v>
+      </c>
+      <c r="G201" s="13" t="s">
         <v>1024</v>
-      </c>
-      <c r="F201" s="13" t="s">
-        <v>995</v>
-      </c>
-      <c r="G201" s="13" t="s">
-        <v>1025</v>
       </c>
       <c r="H201" s="13" t="s">
         <v>133</v>
@@ -12038,7 +12037,7 @@
     </row>
     <row r="202" spans="2:11" ht="41.4" thickBot="1">
       <c r="B202" s="14" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>135</v>
@@ -12047,13 +12046,13 @@
         <v>2022</v>
       </c>
       <c r="E202" s="13" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F202" s="13" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G202" s="13" t="s">
         <v>1027</v>
-      </c>
-      <c r="F202" s="13" t="s">
-        <v>1015</v>
-      </c>
-      <c r="G202" s="13" t="s">
-        <v>1028</v>
       </c>
       <c r="H202" s="13" t="s">
         <v>133</v>
@@ -12070,7 +12069,7 @@
     </row>
     <row r="203" spans="2:11" ht="41.4" thickBot="1">
       <c r="B203" s="14" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>18</v>
@@ -12079,16 +12078,16 @@
         <v>2022</v>
       </c>
       <c r="E203" s="13" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F203" s="13" t="s">
         <v>1030</v>
       </c>
-      <c r="F203" s="13" t="s">
+      <c r="G203" s="13" t="s">
         <v>1031</v>
       </c>
-      <c r="G203" s="13" t="s">
+      <c r="H203" s="13" t="s">
         <v>1032</v>
-      </c>
-      <c r="H203" s="13" t="s">
-        <v>1033</v>
       </c>
       <c r="I203" s="13" t="s">
         <v>845</v>
@@ -12102,7 +12101,7 @@
     </row>
     <row r="204" spans="2:11" ht="31.2" thickBot="1">
       <c r="B204" s="14" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>18</v>
@@ -12111,13 +12110,13 @@
         <v>2018</v>
       </c>
       <c r="E204" s="13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F204" s="13" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G204" s="13" t="s">
         <v>1035</v>
-      </c>
-      <c r="F204" s="13" t="s">
-        <v>1015</v>
-      </c>
-      <c r="G204" s="13" t="s">
-        <v>1036</v>
       </c>
       <c r="H204" s="13" t="s">
         <v>133</v>
@@ -12134,7 +12133,7 @@
     </row>
     <row r="205" spans="2:11" ht="31.2" thickBot="1">
       <c r="B205" s="14" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>135</v>
@@ -12143,16 +12142,16 @@
         <v>2022</v>
       </c>
       <c r="E205" s="13" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F205" s="13" t="s">
         <v>1038</v>
       </c>
-      <c r="F205" s="13" t="s">
+      <c r="G205" s="13" t="s">
         <v>1039</v>
       </c>
-      <c r="G205" s="13" t="s">
+      <c r="H205" s="13" t="s">
         <v>1040</v>
-      </c>
-      <c r="H205" s="13" t="s">
-        <v>1041</v>
       </c>
       <c r="I205" s="13" t="s">
         <v>845</v>
@@ -12166,7 +12165,7 @@
     </row>
     <row r="206" spans="2:11" ht="41.4" thickBot="1">
       <c r="B206" s="14" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>135</v>
@@ -12175,19 +12174,19 @@
         <v>2021</v>
       </c>
       <c r="E206" s="13" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F206" s="13" t="s">
         <v>1043</v>
       </c>
-      <c r="F206" s="13" t="s">
+      <c r="G206" s="13" t="s">
         <v>1044</v>
       </c>
-      <c r="G206" s="13" t="s">
+      <c r="H206" s="13" t="s">
         <v>1045</v>
       </c>
-      <c r="H206" s="13" t="s">
-        <v>1046</v>
-      </c>
       <c r="I206" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J206" s="13">
         <v>5</v>
@@ -12198,7 +12197,7 @@
     </row>
     <row r="207" spans="2:11" ht="31.2" thickBot="1">
       <c r="B207" s="14" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>135</v>
@@ -12207,19 +12206,19 @@
         <v>2020</v>
       </c>
       <c r="E207" s="13" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F207" s="13" t="s">
         <v>1048</v>
       </c>
-      <c r="F207" s="13" t="s">
+      <c r="G207" s="13" t="s">
         <v>1049</v>
       </c>
-      <c r="G207" s="13" t="s">
-        <v>1050</v>
-      </c>
       <c r="H207" s="13" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I207" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J207" s="13">
         <v>4</v>
@@ -12230,7 +12229,7 @@
     </row>
     <row r="208" spans="2:11" ht="31.2" thickBot="1">
       <c r="B208" s="14" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>18</v>
@@ -12239,13 +12238,13 @@
         <v>2018</v>
       </c>
       <c r="E208" s="13" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F208" s="13" t="s">
         <v>1052</v>
       </c>
-      <c r="F208" s="13" t="s">
+      <c r="G208" s="13" t="s">
         <v>1053</v>
-      </c>
-      <c r="G208" s="13" t="s">
-        <v>1054</v>
       </c>
       <c r="H208" s="13" t="s">
         <v>133</v>
@@ -12262,25 +12261,25 @@
     </row>
     <row r="209" spans="2:11" ht="41.4" thickBot="1">
       <c r="B209" s="14" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D209" s="13">
         <v>2021</v>
       </c>
       <c r="E209" s="13" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F209" s="13" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G209" s="13" t="s">
         <v>1056</v>
       </c>
-      <c r="G209" s="13" t="s">
+      <c r="H209" s="13" t="s">
         <v>1057</v>
-      </c>
-      <c r="H209" s="13" t="s">
-        <v>1058</v>
       </c>
       <c r="I209" s="13" t="s">
         <v>845</v>
@@ -12297,19 +12296,19 @@
         <v>356</v>
       </c>
       <c r="C210" s="13" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D210" s="13">
         <v>2022</v>
       </c>
       <c r="E210" s="13" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F210" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G210" s="13" t="s">
         <v>1060</v>
-      </c>
-      <c r="F210" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G210" s="13" t="s">
-        <v>1061</v>
       </c>
       <c r="H210" s="13" t="s">
         <v>131</v>
@@ -12326,22 +12325,22 @@
     </row>
     <row r="211" spans="2:11" ht="41.4" thickBot="1">
       <c r="B211" s="14" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C211" s="13" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D211" s="13">
         <v>2022</v>
       </c>
       <c r="E211" s="13" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F211" s="13" t="s">
         <v>1063</v>
       </c>
-      <c r="F211" s="13" t="s">
+      <c r="G211" s="13" t="s">
         <v>1064</v>
-      </c>
-      <c r="G211" s="13" t="s">
-        <v>1065</v>
       </c>
       <c r="H211" s="13" t="s">
         <v>133</v>
@@ -12361,22 +12360,22 @@
         <v>373</v>
       </c>
       <c r="C212" s="13" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D212" s="13">
         <v>2019</v>
       </c>
       <c r="E212" s="13" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F212" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G212" s="13" t="s">
         <v>1066</v>
       </c>
-      <c r="F212" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G212" s="13" t="s">
+      <c r="H212" s="13" t="s">
         <v>1067</v>
-      </c>
-      <c r="H212" s="13" t="s">
-        <v>1068</v>
       </c>
       <c r="I212" s="13" t="s">
         <v>845</v>
@@ -12390,25 +12389,25 @@
     </row>
     <row r="213" spans="2:11" ht="41.4" thickBot="1">
       <c r="B213" s="14" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C213" s="13" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D213" s="13">
         <v>2022</v>
       </c>
       <c r="E213" s="13" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F213" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G213" s="13" t="s">
         <v>1070</v>
       </c>
-      <c r="F213" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G213" s="13" t="s">
+      <c r="H213" s="13" t="s">
         <v>1071</v>
-      </c>
-      <c r="H213" s="13" t="s">
-        <v>1072</v>
       </c>
       <c r="I213" s="13" t="s">
         <v>845</v>
@@ -12422,7 +12421,7 @@
     </row>
     <row r="214" spans="2:11" ht="41.4" thickBot="1">
       <c r="B214" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>18</v>
@@ -12431,16 +12430,16 @@
         <v>2018</v>
       </c>
       <c r="E214" s="13" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F214" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G214" s="13" t="s">
         <v>1074</v>
       </c>
-      <c r="F214" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G214" s="13" t="s">
+      <c r="H214" s="13" t="s">
         <v>1075</v>
-      </c>
-      <c r="H214" s="13" t="s">
-        <v>1076</v>
       </c>
       <c r="I214" s="13" t="s">
         <v>845</v>
@@ -12454,7 +12453,7 @@
     </row>
     <row r="215" spans="2:11" ht="31.2" thickBot="1">
       <c r="B215" s="14" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>18</v>
@@ -12463,16 +12462,16 @@
         <v>2018</v>
       </c>
       <c r="E215" s="13" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F215" s="13" t="s">
+        <v>975</v>
+      </c>
+      <c r="G215" s="13" t="s">
         <v>1078</v>
       </c>
-      <c r="F215" s="13" t="s">
-        <v>976</v>
-      </c>
-      <c r="G215" s="13" t="s">
-        <v>1079</v>
-      </c>
       <c r="H215" s="13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="I215" s="13" t="s">
         <v>845</v>
@@ -12486,7 +12485,7 @@
     </row>
     <row r="216" spans="2:11" ht="41.4" thickBot="1">
       <c r="B216" s="14" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>135</v>
@@ -12495,16 +12494,16 @@
         <v>2021</v>
       </c>
       <c r="E216" s="13" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F216" s="13" t="s">
         <v>1081</v>
       </c>
-      <c r="F216" s="13" t="s">
+      <c r="G216" s="13" t="s">
         <v>1082</v>
       </c>
-      <c r="G216" s="13" t="s">
-        <v>1083</v>
-      </c>
       <c r="H216" s="13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="I216" s="13" t="s">
         <v>845</v>
@@ -12518,7 +12517,7 @@
     </row>
     <row r="217" spans="2:11" ht="41.4" thickBot="1">
       <c r="B217" s="14" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>135</v>
@@ -12527,16 +12526,16 @@
         <v>2024</v>
       </c>
       <c r="E217" s="13" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F217" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G217" s="13" t="s">
         <v>1085</v>
       </c>
-      <c r="F217" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G217" s="13" t="s">
-        <v>1086</v>
-      </c>
       <c r="H217" s="13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="I217" s="13" t="s">
         <v>845</v>
@@ -12550,7 +12549,7 @@
     </row>
     <row r="218" spans="2:11" ht="41.4" thickBot="1">
       <c r="B218" s="14" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>18</v>
@@ -12559,13 +12558,13 @@
         <v>2024</v>
       </c>
       <c r="E218" s="13" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F218" s="13" t="s">
         <v>1088</v>
       </c>
-      <c r="F218" s="13" t="s">
+      <c r="G218" s="13" t="s">
         <v>1089</v>
-      </c>
-      <c r="G218" s="13" t="s">
-        <v>1090</v>
       </c>
       <c r="H218" s="13" t="s">
         <v>133</v>
@@ -12582,7 +12581,7 @@
     </row>
     <row r="219" spans="2:11" ht="31.2" thickBot="1">
       <c r="B219" s="14" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>18</v>
@@ -12591,13 +12590,13 @@
         <v>2020</v>
       </c>
       <c r="E219" s="13" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F219" s="13" t="s">
         <v>1092</v>
       </c>
-      <c r="F219" s="13" t="s">
+      <c r="G219" s="13" t="s">
         <v>1093</v>
-      </c>
-      <c r="G219" s="13" t="s">
-        <v>1094</v>
       </c>
       <c r="H219" s="13" t="s">
         <v>133</v>
@@ -12614,7 +12613,7 @@
     </row>
     <row r="220" spans="2:11" ht="41.4" thickBot="1">
       <c r="B220" s="14" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>18</v>
@@ -12623,13 +12622,13 @@
         <v>2022</v>
       </c>
       <c r="E220" s="13" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="F220" s="13" t="s">
         <v>216</v>
       </c>
       <c r="G220" s="13" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H220" s="13" t="s">
         <v>133</v>
@@ -12646,7 +12645,7 @@
     </row>
     <row r="221" spans="2:11" ht="41.4" thickBot="1">
       <c r="B221" s="14" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>18</v>
@@ -12655,13 +12654,13 @@
         <v>2022</v>
       </c>
       <c r="E221" s="13" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="F221" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G221" s="13" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="H221" s="13" t="s">
         <v>133</v>
@@ -12678,7 +12677,7 @@
     </row>
     <row r="222" spans="2:11" ht="31.2" thickBot="1">
       <c r="B222" s="14" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>135</v>
@@ -12687,16 +12686,16 @@
         <v>2023</v>
       </c>
       <c r="E222" s="13" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F222" s="13" t="s">
         <v>1102</v>
       </c>
-      <c r="F222" s="13" t="s">
+      <c r="G222" s="13" t="s">
         <v>1103</v>
       </c>
-      <c r="G222" s="13" t="s">
+      <c r="H222" s="13" t="s">
         <v>1104</v>
-      </c>
-      <c r="H222" s="13" t="s">
-        <v>1105</v>
       </c>
       <c r="I222" s="13" t="s">
         <v>845</v>
@@ -12710,7 +12709,7 @@
     </row>
     <row r="223" spans="2:11" ht="41.4" thickBot="1">
       <c r="B223" s="14" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>18</v>
@@ -12719,13 +12718,13 @@
         <v>2021</v>
       </c>
       <c r="E223" s="13" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="F223" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G223" s="13" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="H223" s="13" t="s">
         <v>568</v>
@@ -12742,7 +12741,7 @@
     </row>
     <row r="224" spans="2:11" ht="51.6" thickBot="1">
       <c r="B224" s="14" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>135</v>
@@ -12751,13 +12750,13 @@
         <v>2022</v>
       </c>
       <c r="E224" s="13" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F224" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G224" s="13" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="H224" s="13" t="s">
         <v>133</v>
@@ -12774,7 +12773,7 @@
     </row>
     <row r="225" spans="2:11" ht="41.4" thickBot="1">
       <c r="B225" s="14" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>135</v>
@@ -12783,16 +12782,16 @@
         <v>2024</v>
       </c>
       <c r="E225" s="13" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F225" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G225" s="13" t="s">
+        <v>1113</v>
+      </c>
+      <c r="H225" s="13" t="s">
         <v>1114</v>
-      </c>
-      <c r="H225" s="13" t="s">
-        <v>1115</v>
       </c>
       <c r="I225" s="13" t="s">
         <v>845</v>
@@ -12806,7 +12805,7 @@
     </row>
     <row r="226" spans="2:11" ht="31.2" thickBot="1">
       <c r="B226" s="14" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>18</v>
@@ -12815,13 +12814,13 @@
         <v>2018</v>
       </c>
       <c r="E226" s="13" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F226" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G226" s="13" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="H226" s="13" t="s">
         <v>133</v>
@@ -12838,7 +12837,7 @@
     </row>
     <row r="227" spans="2:11" ht="41.4" thickBot="1">
       <c r="B227" s="14" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>135</v>
@@ -12847,13 +12846,13 @@
         <v>2023</v>
       </c>
       <c r="E227" s="13" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F227" s="13" t="s">
         <v>1120</v>
       </c>
-      <c r="F227" s="13" t="s">
+      <c r="G227" s="13" t="s">
         <v>1121</v>
-      </c>
-      <c r="G227" s="13" t="s">
-        <v>1122</v>
       </c>
       <c r="H227" s="13" t="s">
         <v>133</v>
@@ -12870,7 +12869,7 @@
     </row>
     <row r="228" spans="2:11" ht="41.4" thickBot="1">
       <c r="B228" s="14" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>135</v>
@@ -12879,13 +12878,13 @@
         <v>2024</v>
       </c>
       <c r="E228" s="13" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F228" s="13" t="s">
+        <v>975</v>
+      </c>
+      <c r="G228" s="13" t="s">
         <v>1124</v>
-      </c>
-      <c r="F228" s="13" t="s">
-        <v>976</v>
-      </c>
-      <c r="G228" s="13" t="s">
-        <v>1125</v>
       </c>
       <c r="H228" s="13" t="s">
         <v>133</v>
@@ -12902,7 +12901,7 @@
     </row>
     <row r="229" spans="2:11" ht="51.6" thickBot="1">
       <c r="B229" s="14" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>18</v>
@@ -12911,13 +12910,13 @@
         <v>2022</v>
       </c>
       <c r="E229" s="13" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="F229" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G229" s="13" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="H229" s="13" t="s">
         <v>133</v>
@@ -12934,7 +12933,7 @@
     </row>
     <row r="230" spans="2:11" ht="51.6" thickBot="1">
       <c r="B230" s="14" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>135</v>
@@ -12943,19 +12942,19 @@
         <v>2024</v>
       </c>
       <c r="E230" s="13" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F230" s="13" t="s">
         <v>1130</v>
       </c>
-      <c r="F230" s="13" t="s">
+      <c r="G230" s="13" t="s">
         <v>1131</v>
-      </c>
-      <c r="G230" s="13" t="s">
-        <v>1132</v>
       </c>
       <c r="H230" s="13" t="s">
         <v>133</v>
       </c>
       <c r="I230" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J230" s="13">
         <v>5</v>
@@ -12966,7 +12965,7 @@
     </row>
     <row r="231" spans="2:11" ht="61.8" thickBot="1">
       <c r="B231" s="14" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>18</v>
@@ -12975,13 +12974,13 @@
         <v>2018</v>
       </c>
       <c r="E231" s="13" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F231" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G231" s="13" t="s">
         <v>1134</v>
-      </c>
-      <c r="F231" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G231" s="13" t="s">
-        <v>1135</v>
       </c>
       <c r="H231" s="13" t="s">
         <v>131</v>
@@ -12998,7 +12997,7 @@
     </row>
     <row r="232" spans="2:11" ht="72" thickBot="1">
       <c r="B232" s="14" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>18</v>
@@ -13007,13 +13006,13 @@
         <v>2015</v>
       </c>
       <c r="E232" s="13" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F232" s="13" t="s">
         <v>1137</v>
       </c>
-      <c r="F232" s="13" t="s">
+      <c r="G232" s="13" t="s">
         <v>1138</v>
-      </c>
-      <c r="G232" s="13" t="s">
-        <v>1139</v>
       </c>
       <c r="H232" s="13" t="s">
         <v>133</v>
@@ -13030,7 +13029,7 @@
     </row>
     <row r="233" spans="2:11" ht="61.8" thickBot="1">
       <c r="B233" s="14" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>18</v>
@@ -13039,13 +13038,13 @@
         <v>2023</v>
       </c>
       <c r="E233" s="13" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F233" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G233" s="13" t="s">
         <v>1141</v>
-      </c>
-      <c r="F233" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G233" s="13" t="s">
-        <v>1142</v>
       </c>
       <c r="H233" s="13" t="s">
         <v>133</v>
@@ -13062,7 +13061,7 @@
     </row>
     <row r="234" spans="2:11" ht="51.6" thickBot="1">
       <c r="B234" s="14" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>18</v>
@@ -13071,19 +13070,19 @@
         <v>2024</v>
       </c>
       <c r="E234" s="13" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F234" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G234" s="13" t="s">
         <v>1144</v>
-      </c>
-      <c r="F234" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G234" s="13" t="s">
-        <v>1145</v>
       </c>
       <c r="H234" s="13" t="s">
         <v>133</v>
       </c>
       <c r="I234" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J234" s="13">
         <v>5</v>
@@ -13094,7 +13093,7 @@
     </row>
     <row r="235" spans="2:11" ht="51.6" thickBot="1">
       <c r="B235" s="14" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>18</v>
@@ -13103,19 +13102,19 @@
         <v>2018</v>
       </c>
       <c r="E235" s="13" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F235" s="13" t="s">
         <v>1147</v>
       </c>
-      <c r="F235" s="13" t="s">
+      <c r="G235" s="13" t="s">
         <v>1148</v>
-      </c>
-      <c r="G235" s="13" t="s">
-        <v>1149</v>
       </c>
       <c r="H235" s="13" t="s">
         <v>133</v>
       </c>
       <c r="I235" s="13" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J235" s="13">
         <v>5</v>
@@ -13126,7 +13125,7 @@
     </row>
     <row r="236" spans="2:11" ht="41.4" thickBot="1">
       <c r="B236" s="14" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C236" s="13" t="s">
         <v>851</v>
@@ -13135,13 +13134,13 @@
         <v>2023</v>
       </c>
       <c r="E236" s="13" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F236" s="13" t="s">
         <v>1152</v>
       </c>
-      <c r="F236" s="13" t="s">
+      <c r="G236" s="13" t="s">
         <v>1153</v>
-      </c>
-      <c r="G236" s="13" t="s">
-        <v>1154</v>
       </c>
       <c r="H236" s="13" t="s">
         <v>133</v>
@@ -13158,7 +13157,7 @@
     </row>
     <row r="237" spans="2:11" ht="51.6" thickBot="1">
       <c r="B237" s="14" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>18</v>
@@ -13167,16 +13166,16 @@
         <v>2020</v>
       </c>
       <c r="E237" s="13" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F237" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G237" s="13" t="s">
         <v>1156</v>
       </c>
-      <c r="F237" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G237" s="13" t="s">
-        <v>1157</v>
-      </c>
       <c r="H237" s="13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="I237" s="13" t="s">
         <v>845</v>
@@ -13190,7 +13189,7 @@
     </row>
     <row r="238" spans="2:11" ht="51.6" thickBot="1">
       <c r="B238" s="14" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>18</v>
@@ -13199,16 +13198,16 @@
         <v>2022</v>
       </c>
       <c r="E238" s="13" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F238" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G238" s="13" t="s">
         <v>1159</v>
       </c>
-      <c r="F238" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G238" s="13" t="s">
+      <c r="H238" s="13" t="s">
         <v>1160</v>
-      </c>
-      <c r="H238" s="13" t="s">
-        <v>1161</v>
       </c>
       <c r="I238" s="13" t="s">
         <v>845</v>
@@ -13222,7 +13221,7 @@
     </row>
     <row r="239" spans="2:11" ht="31.2" thickBot="1">
       <c r="B239" s="14" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>135</v>
@@ -13231,13 +13230,13 @@
         <v>2023</v>
       </c>
       <c r="E239" s="13" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F239" s="13" t="s">
         <v>1163</v>
       </c>
-      <c r="F239" s="13" t="s">
+      <c r="G239" s="13" t="s">
         <v>1164</v>
-      </c>
-      <c r="G239" s="13" t="s">
-        <v>1165</v>
       </c>
       <c r="H239" s="13" t="s">
         <v>133</v>
@@ -13254,7 +13253,7 @@
     </row>
     <row r="240" spans="2:11" ht="31.2" thickBot="1">
       <c r="B240" s="14" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>18</v>
@@ -13263,13 +13262,13 @@
         <v>2022</v>
       </c>
       <c r="E240" s="13" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F240" s="13" t="s">
         <v>1167</v>
       </c>
-      <c r="F240" s="13" t="s">
+      <c r="G240" s="13" t="s">
         <v>1168</v>
-      </c>
-      <c r="G240" s="13" t="s">
-        <v>1169</v>
       </c>
       <c r="H240" s="13" t="s">
         <v>522</v>
@@ -13286,7 +13285,7 @@
     </row>
     <row r="241" spans="2:11" ht="31.2" thickBot="1">
       <c r="B241" s="14" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>18</v>
@@ -13295,19 +13294,19 @@
         <v>2019</v>
       </c>
       <c r="E241" s="13" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F241" s="13" t="s">
         <v>1171</v>
       </c>
-      <c r="F241" s="13" t="s">
+      <c r="G241" s="13" t="s">
         <v>1172</v>
-      </c>
-      <c r="G241" s="13" t="s">
-        <v>1173</v>
       </c>
       <c r="H241" s="13" t="s">
         <v>522</v>
       </c>
       <c r="I241" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J241" s="13">
         <v>4</v>
@@ -13318,25 +13317,25 @@
     </row>
     <row r="242" spans="2:11" ht="31.2" thickBot="1">
       <c r="B242" s="14" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D242" s="13">
         <v>2022</v>
       </c>
       <c r="E242" s="13" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F242" s="13" t="s">
+        <v>975</v>
+      </c>
+      <c r="G242" s="13" t="s">
         <v>1175</v>
       </c>
-      <c r="F242" s="13" t="s">
-        <v>976</v>
-      </c>
-      <c r="G242" s="13" t="s">
+      <c r="H242" s="13" t="s">
         <v>1176</v>
-      </c>
-      <c r="H242" s="13" t="s">
-        <v>1177</v>
       </c>
       <c r="I242" s="13" t="s">
         <v>845</v>
@@ -13350,7 +13349,7 @@
     </row>
     <row r="243" spans="2:11" ht="31.2" thickBot="1">
       <c r="B243" s="14" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>18</v>
@@ -13359,16 +13358,16 @@
         <v>2023</v>
       </c>
       <c r="E243" s="13" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="F243" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G243" s="13" t="s">
+        <v>1179</v>
+      </c>
+      <c r="H243" s="13" t="s">
         <v>1180</v>
-      </c>
-      <c r="H243" s="13" t="s">
-        <v>1181</v>
       </c>
       <c r="I243" s="13" t="s">
         <v>845</v>
@@ -13382,7 +13381,7 @@
     </row>
     <row r="244" spans="2:11" ht="28.2" thickBot="1">
       <c r="B244" s="14" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>18</v>
@@ -13391,19 +13390,19 @@
         <v>2015</v>
       </c>
       <c r="E244" s="13" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="F244" s="13" t="s">
         <v>216</v>
       </c>
       <c r="G244" s="13" t="s">
+        <v>1183</v>
+      </c>
+      <c r="H244" s="13" t="s">
         <v>1184</v>
       </c>
-      <c r="H244" s="13" t="s">
-        <v>1185</v>
-      </c>
       <c r="I244" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J244" s="13">
         <v>5</v>
@@ -13414,7 +13413,7 @@
     </row>
     <row r="245" spans="2:11" ht="21" thickBot="1">
       <c r="B245" s="14" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>135</v>
@@ -13423,13 +13422,13 @@
         <v>2024</v>
       </c>
       <c r="E245" s="13" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F245" s="13" t="s">
+        <v>975</v>
+      </c>
+      <c r="G245" s="13" t="s">
         <v>1187</v>
-      </c>
-      <c r="F245" s="13" t="s">
-        <v>976</v>
-      </c>
-      <c r="G245" s="13" t="s">
-        <v>1188</v>
       </c>
       <c r="H245" s="13" t="s">
         <v>522</v>
@@ -13446,7 +13445,7 @@
     </row>
     <row r="246" spans="2:11" ht="31.2" thickBot="1">
       <c r="B246" s="14" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>135</v>
@@ -13455,19 +13454,19 @@
         <v>2018</v>
       </c>
       <c r="E246" s="13" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F246" s="13" t="s">
         <v>1190</v>
       </c>
-      <c r="F246" s="13" t="s">
+      <c r="G246" s="13" t="s">
         <v>1191</v>
-      </c>
-      <c r="G246" s="13" t="s">
-        <v>1192</v>
       </c>
       <c r="H246" s="13" t="s">
         <v>308</v>
       </c>
       <c r="I246" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J246" s="13">
         <v>4</v>
@@ -13478,7 +13477,7 @@
     </row>
     <row r="247" spans="2:11" ht="31.2" thickBot="1">
       <c r="B247" s="14" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>135</v>
@@ -13487,16 +13486,16 @@
         <v>2018</v>
       </c>
       <c r="E247" s="13" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F247" s="13" t="s">
         <v>1194</v>
       </c>
-      <c r="F247" s="13" t="s">
+      <c r="G247" s="13" t="s">
         <v>1195</v>
       </c>
-      <c r="G247" s="13" t="s">
-        <v>1196</v>
-      </c>
       <c r="H247" s="13" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I247" s="13" t="s">
         <v>845</v>
@@ -13510,7 +13509,7 @@
     </row>
     <row r="248" spans="2:11" ht="31.2" thickBot="1">
       <c r="B248" s="14" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>18</v>
@@ -13519,16 +13518,16 @@
         <v>2021</v>
       </c>
       <c r="E248" s="13" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F248" s="13" t="s">
+        <v>975</v>
+      </c>
+      <c r="G248" s="13" t="s">
         <v>1198</v>
       </c>
-      <c r="F248" s="13" t="s">
-        <v>976</v>
-      </c>
-      <c r="G248" s="13" t="s">
+      <c r="H248" s="13" t="s">
         <v>1199</v>
-      </c>
-      <c r="H248" s="13" t="s">
-        <v>1200</v>
       </c>
       <c r="I248" s="13" t="s">
         <v>845</v>
@@ -13542,7 +13541,7 @@
     </row>
     <row r="249" spans="2:11" ht="31.2" thickBot="1">
       <c r="B249" s="14" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>18</v>
@@ -13551,19 +13550,19 @@
         <v>2024</v>
       </c>
       <c r="E249" s="13" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F249" s="13" t="s">
         <v>1202</v>
       </c>
-      <c r="F249" s="13" t="s">
+      <c r="G249" s="13" t="s">
         <v>1203</v>
-      </c>
-      <c r="G249" s="13" t="s">
-        <v>1204</v>
       </c>
       <c r="H249" s="13" t="s">
         <v>133</v>
       </c>
       <c r="I249" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J249" s="13">
         <v>5</v>
@@ -13583,19 +13582,19 @@
         <v>2019</v>
       </c>
       <c r="E250" s="13" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="F250" s="13" t="s">
         <v>238</v>
       </c>
       <c r="G250" s="13" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="H250" s="13" t="s">
         <v>308</v>
       </c>
       <c r="I250" s="13" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="J250" s="13">
         <v>5</v>
@@ -13606,7 +13605,7 @@
     </row>
     <row r="251" spans="2:11" ht="31.2" thickBot="1">
       <c r="B251" s="14" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>18</v>
@@ -13615,16 +13614,16 @@
         <v>2022</v>
       </c>
       <c r="E251" s="13" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="F251" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G251" s="13" t="s">
+        <v>1208</v>
+      </c>
+      <c r="H251" s="13" t="s">
         <v>1209</v>
-      </c>
-      <c r="H251" s="13" t="s">
-        <v>1210</v>
       </c>
       <c r="I251" s="13" t="s">
         <v>845</v>
@@ -13638,7 +13637,7 @@
     </row>
     <row r="252" spans="2:11" ht="31.2" thickBot="1">
       <c r="B252" s="14" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>18</v>
@@ -13647,16 +13646,16 @@
         <v>2022</v>
       </c>
       <c r="E252" s="13" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="F252" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G252" s="13" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="H252" s="13" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I252" s="13" t="s">
         <v>845</v>
@@ -13670,7 +13669,7 @@
     </row>
     <row r="253" spans="2:11" ht="31.2" thickBot="1">
       <c r="B253" s="14" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>18</v>
@@ -13679,16 +13678,16 @@
         <v>2019</v>
       </c>
       <c r="E253" s="13" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="F253" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G253" s="13" t="s">
+        <v>1215</v>
+      </c>
+      <c r="H253" s="13" t="s">
         <v>1216</v>
-      </c>
-      <c r="H253" s="13" t="s">
-        <v>1217</v>
       </c>
       <c r="I253" s="13" t="s">
         <v>845</v>
@@ -13702,7 +13701,7 @@
     </row>
     <row r="254" spans="2:11" ht="31.2" thickBot="1">
       <c r="B254" s="14" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>135</v>
@@ -13711,13 +13710,13 @@
         <v>2023</v>
       </c>
       <c r="E254" s="13" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="F254" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G254" s="13" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="H254" s="13" t="s">
         <v>133</v>
@@ -13734,7 +13733,7 @@
     </row>
     <row r="255" spans="2:11" ht="31.2" thickBot="1">
       <c r="B255" s="14" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>18</v>
@@ -13743,13 +13742,13 @@
         <v>2018</v>
       </c>
       <c r="E255" s="13" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="F255" s="13" t="s">
         <v>238</v>
       </c>
       <c r="G255" s="13" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H255" s="13" t="s">
         <v>133</v>
@@ -13766,7 +13765,7 @@
     </row>
     <row r="256" spans="2:11" ht="31.2" thickBot="1">
       <c r="B256" s="14" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>135</v>
@@ -13775,16 +13774,16 @@
         <v>2022</v>
       </c>
       <c r="E256" s="13" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="F256" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G256" s="13" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H256" s="13" t="s">
         <v>1226</v>
-      </c>
-      <c r="H256" s="13" t="s">
-        <v>1227</v>
       </c>
       <c r="I256" s="13" t="s">
         <v>755</v>
@@ -13798,7 +13797,7 @@
     </row>
     <row r="257" spans="2:11" ht="31.2" thickBot="1">
       <c r="B257" s="14" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>18</v>
@@ -13807,13 +13806,13 @@
         <v>2022</v>
       </c>
       <c r="E257" s="13" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="F257" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G257" s="13" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="H257" s="13" t="s">
         <v>522</v>
@@ -13830,7 +13829,7 @@
     </row>
     <row r="258" spans="2:11" ht="31.2" thickBot="1">
       <c r="B258" s="14" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>18</v>
@@ -13839,13 +13838,13 @@
         <v>2024</v>
       </c>
       <c r="E258" s="13" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F258" s="13" t="s">
         <v>1202</v>
       </c>
-      <c r="F258" s="13" t="s">
+      <c r="G258" s="13" t="s">
         <v>1203</v>
-      </c>
-      <c r="G258" s="13" t="s">
-        <v>1204</v>
       </c>
       <c r="H258" s="13" t="s">
         <v>133</v>
@@ -13862,7 +13861,7 @@
     </row>
     <row r="259" spans="2:11" ht="41.4" thickBot="1">
       <c r="B259" s="14" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>18</v>
@@ -13871,16 +13870,16 @@
         <v>2018</v>
       </c>
       <c r="E259" s="13" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F259" s="13" t="s">
         <v>1232</v>
       </c>
-      <c r="F259" s="13" t="s">
+      <c r="G259" s="13" t="s">
         <v>1233</v>
       </c>
-      <c r="G259" s="13" t="s">
+      <c r="H259" s="13" t="s">
         <v>1234</v>
-      </c>
-      <c r="H259" s="13" t="s">
-        <v>1235</v>
       </c>
       <c r="I259" s="13" t="s">
         <v>845</v>
@@ -13894,7 +13893,7 @@
     </row>
     <row r="260" spans="2:11" ht="31.2" thickBot="1">
       <c r="B260" s="14" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>18</v>
@@ -13903,16 +13902,16 @@
         <v>2019</v>
       </c>
       <c r="E260" s="13" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F260" s="13" t="s">
         <v>1237</v>
       </c>
-      <c r="F260" s="13" t="s">
+      <c r="G260" s="13" t="s">
         <v>1238</v>
       </c>
-      <c r="G260" s="13" t="s">
+      <c r="H260" s="13" t="s">
         <v>1239</v>
-      </c>
-      <c r="H260" s="13" t="s">
-        <v>1240</v>
       </c>
       <c r="I260" s="13" t="s">
         <v>845</v>
@@ -13926,7 +13925,7 @@
     </row>
     <row r="261" spans="2:11" ht="51.6" thickBot="1">
       <c r="B261" s="14" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>18</v>
@@ -13935,13 +13934,13 @@
         <v>2020</v>
       </c>
       <c r="E261" s="13" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="F261" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G261" s="13" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="H261" s="13" t="s">
         <v>245</v>
@@ -13958,7 +13957,7 @@
     </row>
     <row r="262" spans="2:11" ht="51.6" thickBot="1">
       <c r="B262" s="14" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>135</v>
@@ -13967,13 +13966,13 @@
         <v>2022</v>
       </c>
       <c r="E262" s="13" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="F262" s="13" t="s">
         <v>238</v>
       </c>
       <c r="G262" s="13" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="H262" s="13" t="s">
         <v>133</v>
@@ -13990,7 +13989,7 @@
     </row>
     <row r="263" spans="2:11" ht="41.4" thickBot="1">
       <c r="B263" s="14" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>18</v>
@@ -13999,13 +13998,13 @@
         <v>2021</v>
       </c>
       <c r="E263" s="13" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="F263" s="13" t="s">
         <v>158</v>
       </c>
       <c r="G263" s="13" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="H263" s="13" t="s">
         <v>133</v>
@@ -14022,7 +14021,7 @@
     </row>
     <row r="264" spans="2:11" ht="61.8" thickBot="1">
       <c r="B264" s="14" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>18</v>
@@ -14031,16 +14030,16 @@
         <v>2017</v>
       </c>
       <c r="E264" s="13" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="F264" s="13" t="s">
         <v>238</v>
       </c>
       <c r="G264" s="13" t="s">
+        <v>1251</v>
+      </c>
+      <c r="H264" s="13" t="s">
         <v>1252</v>
-      </c>
-      <c r="H264" s="13" t="s">
-        <v>1253</v>
       </c>
       <c r="I264" s="13" t="s">
         <v>845</v>
@@ -14054,7 +14053,7 @@
     </row>
     <row r="265" spans="2:11" ht="61.8" thickBot="1">
       <c r="B265" s="14" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>18</v>
@@ -14063,16 +14062,16 @@
         <v>2023</v>
       </c>
       <c r="E265" s="13" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F265" s="13" t="s">
         <v>1255</v>
       </c>
-      <c r="F265" s="13" t="s">
+      <c r="G265" s="13" t="s">
         <v>1256</v>
       </c>
-      <c r="G265" s="13" t="s">
+      <c r="H265" s="13" t="s">
         <v>1257</v>
-      </c>
-      <c r="H265" s="13" t="s">
-        <v>1258</v>
       </c>
       <c r="I265" s="13" t="s">
         <v>845</v>
@@ -14086,7 +14085,7 @@
     </row>
     <row r="266" spans="2:11" ht="61.8" thickBot="1">
       <c r="B266" s="14" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>18</v>
@@ -14095,16 +14094,16 @@
         <v>2018</v>
       </c>
       <c r="E266" s="13" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="F266" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G266" s="13" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="H266" s="13" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="I266" s="13" t="s">
         <v>845</v>
@@ -14118,22 +14117,22 @@
     </row>
     <row r="267" spans="2:11" ht="31.2" thickBot="1">
       <c r="B267" s="14" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C267" s="13" t="s">
         <v>1262</v>
-      </c>
-      <c r="C267" s="13" t="s">
-        <v>1263</v>
       </c>
       <c r="D267" s="13">
         <v>2021</v>
       </c>
       <c r="E267" s="13" t="s">
+        <v>1263</v>
+      </c>
+      <c r="F267" s="13" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G267" s="13" t="s">
         <v>1264</v>
-      </c>
-      <c r="F267" s="13" t="s">
-        <v>1191</v>
-      </c>
-      <c r="G267" s="13" t="s">
-        <v>1265</v>
       </c>
       <c r="H267" s="13" t="s">
         <v>133</v>
@@ -14150,22 +14149,22 @@
     </row>
     <row r="268" spans="2:11" ht="31.2" thickBot="1">
       <c r="B268" s="14" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C268" s="13" t="s">
         <v>1266</v>
-      </c>
-      <c r="C268" s="13" t="s">
-        <v>1267</v>
       </c>
       <c r="D268" s="13">
         <v>2019</v>
       </c>
       <c r="E268" s="13" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F268" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G268" s="13" t="s">
         <v>1268</v>
-      </c>
-      <c r="F268" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G268" s="13" t="s">
-        <v>1269</v>
       </c>
       <c r="H268" s="13" t="s">
         <v>133</v>
@@ -14182,28 +14181,28 @@
     </row>
     <row r="269" spans="2:11" ht="41.4" thickBot="1">
       <c r="B269" s="14" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C269" s="13" t="s">
         <v>1270</v>
-      </c>
-      <c r="C269" s="13" t="s">
-        <v>1271</v>
       </c>
       <c r="D269" s="13">
         <v>2023</v>
       </c>
       <c r="E269" s="13" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F269" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G269" s="13" t="s">
         <v>1272</v>
-      </c>
-      <c r="F269" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G269" s="13" t="s">
-        <v>1273</v>
       </c>
       <c r="H269" s="13" t="s">
         <v>131</v>
       </c>
       <c r="I269" s="13" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="J269" s="13">
         <v>4</v>
@@ -14214,7 +14213,7 @@
     </row>
     <row r="270" spans="2:11" ht="31.2" thickBot="1">
       <c r="B270" s="14" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>135</v>
@@ -14223,16 +14222,16 @@
         <v>2021</v>
       </c>
       <c r="E270" s="13" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F270" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G270" s="13" t="s">
         <v>1276</v>
       </c>
-      <c r="F270" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G270" s="13" t="s">
-        <v>1277</v>
-      </c>
       <c r="H270" s="13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="I270" s="13" t="s">
         <v>845</v>
@@ -14246,7 +14245,7 @@
     </row>
     <row r="271" spans="2:11" ht="31.2" thickBot="1">
       <c r="B271" s="14" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>18</v>
@@ -14255,16 +14254,16 @@
         <v>2021</v>
       </c>
       <c r="E271" s="13" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F271" s="13" t="s">
         <v>1279</v>
       </c>
-      <c r="F271" s="13" t="s">
+      <c r="G271" s="13" t="s">
         <v>1280</v>
       </c>
-      <c r="G271" s="13" t="s">
-        <v>1281</v>
-      </c>
       <c r="H271" s="13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="I271" s="13" t="s">
         <v>845</v>
@@ -14278,7 +14277,7 @@
     </row>
     <row r="272" spans="2:11" ht="31.2" thickBot="1">
       <c r="B272" s="14" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>18</v>
@@ -14287,13 +14286,13 @@
         <v>2022</v>
       </c>
       <c r="E272" s="13" t="s">
+        <v>1282</v>
+      </c>
+      <c r="F272" s="13" t="s">
         <v>1283</v>
       </c>
-      <c r="F272" s="13" t="s">
+      <c r="G272" s="13" t="s">
         <v>1284</v>
-      </c>
-      <c r="G272" s="13" t="s">
-        <v>1285</v>
       </c>
       <c r="H272" s="13" t="s">
         <v>133</v>
@@ -14310,7 +14309,7 @@
     </row>
     <row r="273" spans="2:11" ht="82.2" thickBot="1">
       <c r="B273" s="14" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>18</v>
@@ -14319,13 +14318,13 @@
         <v>2019</v>
       </c>
       <c r="E273" s="13" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F273" s="13" t="s">
         <v>1287</v>
       </c>
-      <c r="F273" s="13" t="s">
+      <c r="G273" s="13" t="s">
         <v>1288</v>
-      </c>
-      <c r="G273" s="13" t="s">
-        <v>1289</v>
       </c>
       <c r="H273" s="13" t="s">
         <v>133</v>
@@ -14342,7 +14341,7 @@
     </row>
     <row r="274" spans="2:11" ht="31.2" thickBot="1">
       <c r="B274" s="14" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>18</v>
@@ -14351,16 +14350,16 @@
         <v>2021</v>
       </c>
       <c r="E274" s="13" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F274" s="13" t="s">
         <v>1291</v>
       </c>
-      <c r="F274" s="13" t="s">
+      <c r="G274" s="13" t="s">
         <v>1292</v>
       </c>
-      <c r="G274" s="13" t="s">
-        <v>1293</v>
-      </c>
       <c r="H274" s="13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="I274" s="13" t="s">
         <v>845</v>
@@ -14374,7 +14373,7 @@
     </row>
     <row r="275" spans="2:11" ht="31.2" thickBot="1">
       <c r="B275" s="14" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>18</v>
@@ -14383,16 +14382,16 @@
         <v>2021</v>
       </c>
       <c r="E275" s="13" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F275" s="13" t="s">
         <v>1295</v>
       </c>
-      <c r="F275" s="13" t="s">
+      <c r="G275" s="13" t="s">
         <v>1296</v>
       </c>
-      <c r="G275" s="13" t="s">
-        <v>1297</v>
-      </c>
       <c r="H275" s="13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="I275" s="13" t="s">
         <v>845</v>
@@ -14406,7 +14405,7 @@
     </row>
     <row r="276" spans="2:11" ht="41.4" thickBot="1">
       <c r="B276" s="14" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>18</v>
@@ -14415,13 +14414,13 @@
         <v>2018</v>
       </c>
       <c r="E276" s="13" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F276" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="G276" s="13" t="s">
         <v>1299</v>
-      </c>
-      <c r="F276" s="13" t="s">
-        <v>879</v>
-      </c>
-      <c r="G276" s="13" t="s">
-        <v>1300</v>
       </c>
       <c r="H276" s="13" t="s">
         <v>133</v>
@@ -14438,7 +14437,7 @@
     </row>
     <row r="277" spans="2:11" ht="41.4" thickBot="1">
       <c r="B277" s="14" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>18</v>
@@ -14447,16 +14446,16 @@
         <v>2021</v>
       </c>
       <c r="E277" s="13" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F277" s="13" t="s">
         <v>1302</v>
       </c>
-      <c r="F277" s="13" t="s">
+      <c r="G277" s="13" t="s">
         <v>1303</v>
       </c>
-      <c r="G277" s="13" t="s">
-        <v>1304</v>
-      </c>
       <c r="H277" s="13" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I277" s="13" t="s">
         <v>845</v>

</xml_diff>